<commit_message>
il est tard mes yeux piquent
</commit_message>
<xml_diff>
--- a/card_export.xlsx
+++ b/card_export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\Documents\CodeBlock\Project_SFML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CEBD0A95-E9B2-4B1C-B789-4ABF8CECF15A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EB79FA9F-E4CB-411D-AE36-1C3420EAD20D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="99">
   <si>
     <t>Commun</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>Arbalete automatique</t>
+  </si>
+  <si>
+    <t>Magie</t>
   </si>
 </sst>
 </file>
@@ -672,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -703,6 +706,9 @@
       <c r="H1" s="1">
         <v>1</v>
       </c>
+      <c r="I1" s="1">
+        <v>0</v>
+      </c>
       <c r="J1" s="1">
         <v>0</v>
       </c>
@@ -732,6 +738,9 @@
       <c r="H2" s="1">
         <v>3</v>
       </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
@@ -761,6 +770,9 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
@@ -790,6 +802,9 @@
       <c r="H4" s="1">
         <v>1</v>
       </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
@@ -818,6 +833,9 @@
       </c>
       <c r="H5" s="1">
         <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
@@ -848,6 +866,9 @@
       <c r="H6" s="1">
         <v>2</v>
       </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
@@ -877,6 +898,9 @@
       <c r="H7" s="1">
         <v>2</v>
       </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
@@ -906,6 +930,9 @@
       <c r="H8" s="1">
         <v>3</v>
       </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
       <c r="J8" s="1">
         <v>0</v>
       </c>
@@ -935,6 +962,9 @@
       <c r="H9" s="1">
         <v>1</v>
       </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
       <c r="J9" s="1">
         <v>0</v>
       </c>
@@ -964,6 +994,9 @@
       <c r="H10" s="1">
         <v>1</v>
       </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
       <c r="J10" s="1">
         <v>0</v>
       </c>
@@ -993,6 +1026,9 @@
       <c r="H11" s="1">
         <v>1</v>
       </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
@@ -1022,6 +1058,9 @@
       <c r="H12" s="1">
         <v>4</v>
       </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
@@ -1051,6 +1090,9 @@
       <c r="H13" s="1">
         <v>2</v>
       </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
@@ -1080,6 +1122,9 @@
       <c r="H14" s="1">
         <v>1</v>
       </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
       <c r="J14" s="1">
         <v>0</v>
       </c>
@@ -1109,6 +1154,9 @@
       <c r="H15" s="1">
         <v>3</v>
       </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
       <c r="J15" s="1">
         <v>0</v>
       </c>
@@ -1138,6 +1186,9 @@
       <c r="H16" s="1">
         <v>2</v>
       </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
       <c r="J16" s="1">
         <v>0</v>
       </c>
@@ -1167,6 +1218,9 @@
       <c r="H17" s="1">
         <v>2</v>
       </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
       <c r="J17" s="1">
         <v>0</v>
       </c>
@@ -1196,6 +1250,9 @@
       <c r="H18" s="1">
         <v>1</v>
       </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
       <c r="J18" s="1">
         <v>0</v>
       </c>
@@ -1225,6 +1282,9 @@
       <c r="H19" s="1">
         <v>2</v>
       </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
       <c r="J19" s="1">
         <v>0</v>
       </c>
@@ -1254,6 +1314,9 @@
       <c r="H20" s="1">
         <v>1</v>
       </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
@@ -1283,6 +1346,9 @@
       <c r="H21" s="1">
         <v>1</v>
       </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
@@ -1312,6 +1378,9 @@
       <c r="H22" s="1">
         <v>2</v>
       </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
       <c r="J22" s="1">
         <v>0</v>
       </c>
@@ -1341,6 +1410,9 @@
       <c r="H23" s="1">
         <v>1</v>
       </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
       <c r="J23" s="1">
         <v>0</v>
       </c>
@@ -1370,6 +1442,9 @@
       <c r="H24" s="1">
         <v>1</v>
       </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
       <c r="J24" s="1">
         <v>0</v>
       </c>
@@ -1399,6 +1474,9 @@
       <c r="H25" s="1">
         <v>1</v>
       </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
       <c r="J25" s="1">
         <v>0</v>
       </c>
@@ -1428,6 +1506,9 @@
       <c r="H26" s="1">
         <v>3</v>
       </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
       <c r="J26" s="1">
         <v>0</v>
       </c>
@@ -1457,6 +1538,9 @@
       <c r="H27" s="1">
         <v>2</v>
       </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
       <c r="J27" s="1">
         <v>0</v>
       </c>
@@ -1486,6 +1570,9 @@
       <c r="H28" s="1">
         <v>2</v>
       </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
       <c r="J28" s="1">
         <v>0</v>
       </c>
@@ -1515,6 +1602,9 @@
       <c r="H29" s="1">
         <v>1</v>
       </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
       <c r="J29" s="1">
         <v>0</v>
       </c>
@@ -1544,6 +1634,9 @@
       <c r="H30" s="1">
         <v>3</v>
       </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
       <c r="J30" s="1">
         <v>0</v>
       </c>
@@ -1573,6 +1666,9 @@
       <c r="H31" s="1">
         <v>1</v>
       </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
       <c r="J31" s="1">
         <v>0</v>
       </c>
@@ -1602,6 +1698,9 @@
       <c r="H32" s="1">
         <v>2</v>
       </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
       <c r="J32" s="1">
         <v>0</v>
       </c>
@@ -1631,6 +1730,9 @@
       <c r="H33" s="1">
         <v>2</v>
       </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
       <c r="J33" s="1">
         <v>0</v>
       </c>
@@ -1660,6 +1762,9 @@
       <c r="H34" s="1">
         <v>1</v>
       </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
       <c r="J34" s="1">
         <v>0</v>
       </c>
@@ -1689,6 +1794,9 @@
       <c r="H35" s="1">
         <v>1</v>
       </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
       <c r="J35" s="1">
         <v>0</v>
       </c>
@@ -1718,6 +1826,9 @@
       <c r="H36" s="1">
         <v>2</v>
       </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
       <c r="J36" s="1">
         <v>0</v>
       </c>
@@ -1747,6 +1858,9 @@
       <c r="H37" s="1">
         <v>2</v>
       </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
       <c r="J37" s="1">
         <v>0</v>
       </c>
@@ -1776,6 +1890,9 @@
       <c r="H38" s="1">
         <v>1</v>
       </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
       <c r="J38" s="1">
         <v>0</v>
       </c>
@@ -1805,6 +1922,9 @@
       <c r="H39" s="1">
         <v>1</v>
       </c>
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
       <c r="J39" s="1">
         <v>0</v>
       </c>
@@ -1834,6 +1954,9 @@
       <c r="H40" s="1">
         <v>1</v>
       </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
       <c r="J40" s="1">
         <v>0</v>
       </c>
@@ -1863,6 +1986,9 @@
       <c r="H41" s="1">
         <v>1</v>
       </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
       <c r="J41" s="1">
         <v>0</v>
       </c>
@@ -1892,6 +2018,9 @@
       <c r="H42" s="1">
         <v>3</v>
       </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
       <c r="J42" s="1">
         <v>0</v>
       </c>
@@ -1921,6 +2050,9 @@
       <c r="H43" s="1">
         <v>1</v>
       </c>
+      <c r="I43" s="1">
+        <v>0</v>
+      </c>
       <c r="J43" s="1">
         <v>0</v>
       </c>
@@ -1950,6 +2082,9 @@
       <c r="H44" s="1">
         <v>2</v>
       </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
       <c r="J44" s="1">
         <v>0</v>
       </c>
@@ -1979,6 +2114,9 @@
       <c r="H45" s="1">
         <v>2</v>
       </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
       <c r="J45" s="1">
         <v>0</v>
       </c>
@@ -2008,6 +2146,9 @@
       <c r="H46" s="1">
         <v>2</v>
       </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
       <c r="J46" s="1">
         <v>0</v>
       </c>
@@ -2037,6 +2178,9 @@
       <c r="H47" s="1">
         <v>2</v>
       </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
       <c r="J47" s="1">
         <v>0</v>
       </c>
@@ -2066,6 +2210,9 @@
       <c r="H48" s="1">
         <v>3</v>
       </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
       <c r="J48" s="1">
         <v>0</v>
       </c>
@@ -2095,6 +2242,9 @@
       <c r="H49" s="1">
         <v>1</v>
       </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
       <c r="J49" s="1">
         <v>0</v>
       </c>
@@ -2124,6 +2274,9 @@
       <c r="H50" s="1">
         <v>2</v>
       </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
       <c r="J50" s="1">
         <v>0</v>
       </c>
@@ -2153,6 +2306,9 @@
       <c r="H51" s="1">
         <v>1</v>
       </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
       <c r="J51" s="1">
         <v>0</v>
       </c>
@@ -2711,8 +2867,23 @@
       <c r="C69" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="D69" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E69" s="1">
         <v>1</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
       </c>
       <c r="J69" s="1">
         <v>2</v>
@@ -2728,8 +2899,23 @@
       <c r="C70" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="D70" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E70" s="1">
         <v>2</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0</v>
       </c>
       <c r="J70" s="1">
         <v>2</v>
@@ -2745,8 +2931,23 @@
       <c r="C71" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="D71" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E71" s="1">
         <v>2</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0</v>
       </c>
       <c r="J71" s="1">
         <v>2</v>
@@ -2762,8 +2963,23 @@
       <c r="C72" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="D72" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E72" s="1">
         <v>3</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0</v>
       </c>
       <c r="J72" s="1">
         <v>2</v>
@@ -2779,8 +2995,23 @@
       <c r="C73" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="D73" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E73" s="1">
         <v>3</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0</v>
+      </c>
+      <c r="H73" s="1">
+        <v>0</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0</v>
       </c>
       <c r="J73" s="1">
         <v>2</v>
@@ -2796,8 +3027,23 @@
       <c r="C74" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="D74" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E74" s="1">
         <v>4</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1">
+        <v>0</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0</v>
       </c>
       <c r="J74" s="1">
         <v>2</v>
@@ -2813,8 +3059,23 @@
       <c r="C75" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="D75" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E75" s="1">
         <v>5</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0</v>
       </c>
       <c r="J75" s="1">
         <v>2</v>
@@ -2830,8 +3091,23 @@
       <c r="C76" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="D76" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E76" s="1">
         <v>5</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0</v>
       </c>
       <c r="J76" s="1">
         <v>2</v>
@@ -2847,8 +3123,23 @@
       <c r="C77" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="D77" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E77" s="1">
         <v>5</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0</v>
       </c>
       <c r="J77" s="1">
         <v>2</v>
@@ -2864,6 +3155,24 @@
       <c r="C78" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="D78" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0</v>
+      </c>
       <c r="J78" s="1">
         <v>2</v>
       </c>
@@ -2878,8 +3187,23 @@
       <c r="C79" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="D79" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E79" s="1">
         <v>6</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0</v>
       </c>
       <c r="J79" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
tour et bug case
implémentation des tours, le graphisme sera peut-être à changer, il reste le game over à faire.
Bug du hover des cases corriger, on ne peut plus passer sur plusieurs cases en même temps
</commit_message>
<xml_diff>
--- a/card_export.xlsx
+++ b/card_export.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\Documents\CodeBlock\Project_SFML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B2091EB7-400B-4BEB-8180-DC31E0396527}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6BA6FB39-B8D7-4C60-BB14-10B4FBEE4B32}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="100">
   <si>
     <t>Commun</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Adepte de la lumiere</t>
+  </si>
+  <si>
+    <t>Tour</t>
   </si>
 </sst>
 </file>
@@ -673,58 +676,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1">
-        <v>0</v>
-      </c>
-      <c r="J1" s="1">
-        <v>0</v>
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>15</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>85</v>
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -736,7 +739,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -747,16 +750,16 @@
     </row>
     <row r="3" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -765,10 +768,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -779,22 +782,22 @@
     </row>
     <row r="4" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>2</v>
@@ -811,22 +814,22 @@
     </row>
     <row r="5" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -843,28 +846,28 @@
     </row>
     <row r="6" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
@@ -875,16 +878,16 @@
     </row>
     <row r="7" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>85</v>
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -893,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -907,15 +910,15 @@
     </row>
     <row r="8" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E8" s="1">
@@ -928,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -939,16 +942,16 @@
     </row>
     <row r="9" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -960,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -971,16 +974,16 @@
     </row>
     <row r="10" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -989,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -1003,22 +1006,22 @@
     </row>
     <row r="11" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1">
         <v>3</v>
@@ -1035,28 +1038,28 @@
     </row>
     <row r="12" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
@@ -1067,28 +1070,28 @@
     </row>
     <row r="13" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1">
         <v>3</v>
       </c>
       <c r="F13" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
       </c>
       <c r="H13" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -1099,28 +1102,28 @@
     </row>
     <row r="14" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1">
         <v>3</v>
       </c>
       <c r="F14" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G14" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -1131,16 +1134,16 @@
     </row>
     <row r="15" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1149,10 +1152,10 @@
         <v>2</v>
       </c>
       <c r="G15" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -1163,28 +1166,28 @@
     </row>
     <row r="16" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1">
         <v>3</v>
       </c>
       <c r="F16" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16" s="1">
         <v>3</v>
       </c>
       <c r="H16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
@@ -1195,16 +1198,16 @@
     </row>
     <row r="17" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1">
         <v>3</v>
@@ -1227,28 +1230,28 @@
     </row>
     <row r="18" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
       </c>
       <c r="F18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -1259,19 +1262,19 @@
     </row>
     <row r="19" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
@@ -1280,7 +1283,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -1291,28 +1294,28 @@
     </row>
     <row r="20" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1">
         <v>4</v>
       </c>
       <c r="F20" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -1323,25 +1326,25 @@
     </row>
     <row r="21" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1">
         <v>4</v>
       </c>
       <c r="F21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
@@ -1355,28 +1358,28 @@
     </row>
     <row r="22" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E22" s="1">
         <v>4</v>
       </c>
       <c r="F22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G22" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
@@ -1387,28 +1390,28 @@
     </row>
     <row r="23" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E23" s="1">
         <v>4</v>
       </c>
       <c r="F23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G23" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -1419,25 +1422,25 @@
     </row>
     <row r="24" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1">
         <v>4</v>
       </c>
       <c r="F24" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G24" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
@@ -1451,25 +1454,25 @@
     </row>
     <row r="25" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E25" s="1">
         <v>4</v>
       </c>
       <c r="F25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G25" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H25" s="1">
         <v>1</v>
@@ -1483,28 +1486,28 @@
     </row>
     <row r="26" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E26" s="1">
         <v>4</v>
       </c>
       <c r="F26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G26" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H26" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -1515,28 +1518,28 @@
     </row>
     <row r="27" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E27" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G27" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -1547,25 +1550,25 @@
     </row>
     <row r="28" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1">
         <v>5</v>
       </c>
       <c r="F28" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G28" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H28" s="1">
         <v>2</v>
@@ -1579,28 +1582,28 @@
     </row>
     <row r="29" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E29" s="1">
         <v>5</v>
       </c>
       <c r="F29" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G29" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" s="1">
         <v>0</v>
@@ -1611,28 +1614,28 @@
     </row>
     <row r="30" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E30" s="1">
         <v>5</v>
       </c>
       <c r="F30" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G30" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H30" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
@@ -1643,28 +1646,28 @@
     </row>
     <row r="31" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="E31" s="1">
         <v>5</v>
       </c>
       <c r="F31" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G31" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H31" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
@@ -1675,16 +1678,16 @@
     </row>
     <row r="32" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="E32" s="1">
         <v>5</v>
@@ -1693,10 +1696,10 @@
         <v>3</v>
       </c>
       <c r="G32" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32" s="1">
         <v>0</v>
@@ -1707,13 +1710,13 @@
     </row>
     <row r="33" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>22</v>
@@ -1722,7 +1725,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G33" s="1">
         <v>5</v>
@@ -1739,28 +1742,28 @@
     </row>
     <row r="34" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E34" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" s="1">
         <v>2</v>
       </c>
       <c r="G34" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H34" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
@@ -1771,25 +1774,25 @@
     </row>
     <row r="35" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E35" s="1">
         <v>6</v>
       </c>
       <c r="F35" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G35" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H35" s="1">
         <v>1</v>
@@ -1803,28 +1806,28 @@
     </row>
     <row r="36" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="E36" s="1">
         <v>6</v>
       </c>
       <c r="F36" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G36" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H36" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="1">
         <v>0</v>
@@ -1835,25 +1838,25 @@
     </row>
     <row r="37" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1">
         <v>6</v>
       </c>
       <c r="F37" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G37" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H37" s="1">
         <v>2</v>
@@ -1867,28 +1870,28 @@
     </row>
     <row r="38" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E38" s="1">
         <v>6</v>
       </c>
       <c r="F38" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G38" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H38" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" s="1">
         <v>0</v>
@@ -1899,22 +1902,22 @@
     </row>
     <row r="39" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E39" s="1">
         <v>6</v>
       </c>
       <c r="F39" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G39" s="1">
         <v>6</v>
@@ -1931,13 +1934,13 @@
     </row>
     <row r="40" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>22</v>
@@ -1946,10 +1949,10 @@
         <v>6</v>
       </c>
       <c r="F40" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G40" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H40" s="1">
         <v>1</v>
@@ -1963,25 +1966,25 @@
     </row>
     <row r="41" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E41" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G41" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H41" s="1">
         <v>1</v>
@@ -1995,28 +1998,28 @@
     </row>
     <row r="42" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="E42" s="1">
         <v>7</v>
       </c>
       <c r="F42" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G42" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H42" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42" s="1">
         <v>0</v>
@@ -2027,16 +2030,16 @@
     </row>
     <row r="43" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E43" s="1">
         <v>7</v>
@@ -2045,10 +2048,10 @@
         <v>7</v>
       </c>
       <c r="G43" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H43" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I43" s="1">
         <v>0</v>
@@ -2059,28 +2062,28 @@
     </row>
     <row r="44" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E44" s="1">
         <v>7</v>
       </c>
       <c r="F44" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G44" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H44" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I44" s="1">
         <v>0</v>
@@ -2091,25 +2094,25 @@
     </row>
     <row r="45" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E45" s="1">
         <v>7</v>
       </c>
       <c r="F45" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G45" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H45" s="1">
         <v>2</v>
@@ -2123,25 +2126,25 @@
     </row>
     <row r="46" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="E46" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F46" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G46" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H46" s="1">
         <v>2</v>
@@ -2155,25 +2158,25 @@
     </row>
     <row r="47" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E47" s="1">
         <v>8</v>
       </c>
       <c r="F47" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G47" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H47" s="1">
         <v>2</v>
@@ -2187,28 +2190,28 @@
     </row>
     <row r="48" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="E48" s="1">
         <v>8</v>
       </c>
       <c r="F48" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G48" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H48" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I48" s="1">
         <v>0</v>
@@ -2219,28 +2222,28 @@
     </row>
     <row r="49" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E49" s="1">
         <v>8</v>
       </c>
       <c r="F49" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G49" s="1">
         <v>7</v>
       </c>
       <c r="H49" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I49" s="1">
         <v>0</v>
@@ -2251,28 +2254,28 @@
     </row>
     <row r="50" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E50" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G50" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50" s="1">
         <v>0</v>
@@ -2283,16 +2286,16 @@
     </row>
     <row r="51" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E51" s="1">
         <v>9</v>
@@ -2301,10 +2304,10 @@
         <v>8</v>
       </c>
       <c r="G51" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H51" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I51" s="1">
         <v>0</v>
@@ -2315,51 +2318,51 @@
     </row>
     <row r="52" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E52" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F52" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G52" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="1">
         <v>0</v>
       </c>
       <c r="J52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="E53" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
@@ -2371,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" s="1">
         <v>1</v>
@@ -2379,16 +2382,16 @@
     </row>
     <row r="54" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -2397,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="G54" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H54" s="1">
         <v>0</v>
@@ -2411,25 +2414,25 @@
     </row>
     <row r="55" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E55" s="1">
         <v>3</v>
       </c>
       <c r="F55" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G55" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H55" s="1">
         <v>0</v>
@@ -2443,31 +2446,31 @@
     </row>
     <row r="56" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E56" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G56" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H56" s="1">
         <v>0</v>
       </c>
       <c r="I56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" s="1">
         <v>1</v>
@@ -2475,16 +2478,16 @@
     </row>
     <row r="57" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E57" s="1">
         <v>4</v>
@@ -2493,13 +2496,13 @@
         <v>0</v>
       </c>
       <c r="G57" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H57" s="1">
         <v>0</v>
       </c>
       <c r="I57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" s="1">
         <v>1</v>
@@ -2507,16 +2510,16 @@
     </row>
     <row r="58" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -2525,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H58" s="1">
         <v>0</v>
@@ -2539,16 +2542,16 @@
     </row>
     <row r="59" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="E59" s="1">
         <v>4</v>
@@ -2571,22 +2574,22 @@
     </row>
     <row r="60" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="E60" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G60" s="1">
         <v>6</v>
@@ -2603,25 +2606,25 @@
     </row>
     <row r="61" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E61" s="1">
         <v>5</v>
       </c>
       <c r="F61" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G61" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H61" s="1">
         <v>0</v>
@@ -2635,25 +2638,25 @@
     </row>
     <row r="62" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E62" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
       </c>
       <c r="G62" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H62" s="1">
         <v>0</v>
@@ -2667,25 +2670,25 @@
     </row>
     <row r="63" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="E63" s="1">
         <v>6</v>
       </c>
       <c r="F63" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G63" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H63" s="1">
         <v>0</v>
@@ -2699,31 +2702,31 @@
     </row>
     <row r="64" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="E64" s="1">
         <v>6</v>
       </c>
       <c r="F64" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G64" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H64" s="1">
         <v>0</v>
       </c>
       <c r="I64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" s="1">
         <v>1</v>
@@ -2731,31 +2734,31 @@
     </row>
     <row r="65" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="E65" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" s="1">
         <v>0</v>
       </c>
       <c r="G65" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H65" s="1">
         <v>0</v>
       </c>
       <c r="I65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J65" s="1">
         <v>1</v>
@@ -2763,31 +2766,31 @@
     </row>
     <row r="66" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E66" s="1">
+        <v>7</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
         <v>8</v>
       </c>
-      <c r="F66" s="1">
-        <v>0</v>
-      </c>
-      <c r="G66" s="1">
-        <v>10</v>
-      </c>
       <c r="H66" s="1">
         <v>0</v>
       </c>
       <c r="I66" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J66" s="1">
         <v>1</v>
@@ -2795,31 +2798,31 @@
     </row>
     <row r="67" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E67" s="1">
         <v>8</v>
       </c>
       <c r="F67" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G67" s="1">
         <v>10</v>
       </c>
       <c r="H67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J67" s="1">
         <v>1</v>
@@ -2827,25 +2830,25 @@
     </row>
     <row r="68" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E68" s="1">
+        <v>8</v>
+      </c>
+      <c r="F68" s="1">
+        <v>6</v>
+      </c>
+      <c r="G68" s="1">
         <v>10</v>
-      </c>
-      <c r="F68" s="1">
-        <v>15</v>
-      </c>
-      <c r="G68" s="1">
-        <v>20</v>
       </c>
       <c r="H68" s="1">
         <v>1</v>
@@ -2859,51 +2862,51 @@
     </row>
     <row r="69" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="E69" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G69" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E70" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
@@ -2923,13 +2926,13 @@
     </row>
     <row r="71" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>97</v>
@@ -2955,19 +2958,19 @@
     </row>
     <row r="72" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E72" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" s="1">
         <v>0</v>
@@ -2987,13 +2990,13 @@
     </row>
     <row r="73" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>97</v>
@@ -3019,19 +3022,19 @@
     </row>
     <row r="74" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E74" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" s="1">
         <v>0</v>
@@ -3051,19 +3054,19 @@
     </row>
     <row r="75" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E75" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" s="1">
         <v>0</v>
@@ -3083,13 +3086,13 @@
     </row>
     <row r="76" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>97</v>
@@ -3115,13 +3118,13 @@
     </row>
     <row r="77" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>97</v>
@@ -3147,19 +3150,19 @@
     </row>
     <row r="78" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E78" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F78" s="1">
         <v>0</v>
@@ -3179,33 +3182,65 @@
     </row>
     <row r="79" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E79" s="1">
+        <v>0</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0</v>
+      </c>
+      <c r="J79" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E80" s="1">
         <v>6</v>
       </c>
-      <c r="F79" s="1">
-        <v>0</v>
-      </c>
-      <c r="G79" s="1">
-        <v>0</v>
-      </c>
-      <c r="H79" s="1">
-        <v>0</v>
-      </c>
-      <c r="I79" s="1">
-        <v>0</v>
-      </c>
-      <c r="J79" s="1">
+      <c r="F80" s="1">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0</v>
+      </c>
+      <c r="J80" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bug mort des cartes, fin de partie sans arret de jeux
</commit_message>
<xml_diff>
--- a/card_export.xlsx
+++ b/card_export.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\Documents\CodeBlock\Project_SFML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6BA6FB39-B8D7-4C60-BB14-10B4FBEE4B32}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9DE55941-FDFC-42C1-A460-CF303B6C00B0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,7 +679,7 @@
   <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>

</xml_diff>